<commit_message>
Created group_score function and updated data file.
</commit_message>
<xml_diff>
--- a/thesis_data.xlsx
+++ b/thesis_data.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emma\Documents\Mocku_for_change_data_analisys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emma\Documents\Mocku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C03D5F-2640-43CF-895D-BFA9A87CF95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5028F336-D2E8-4998-9E33-D39FC6740AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15852" yWindow="2820" windowWidth="7188" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="temi" sheetId="1" r:id="rId1"/>
     <sheet name="tensioni" sheetId="4" r:id="rId2"/>
-    <sheet name="Condizioni" sheetId="2" r:id="rId3"/>
-    <sheet name="Punteggio" sheetId="3" r:id="rId4"/>
+    <sheet name="caratteristiche" sheetId="2" r:id="rId3"/>
+    <sheet name="punteggio" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="55">
   <si>
     <t>Gruppo</t>
   </si>
@@ -144,57 +144,6 @@
     <t xml:space="preserve">Debole </t>
   </si>
   <si>
-    <t>temi presenti in intenzioni</t>
-  </si>
-  <si>
-    <t>temi presenti in risultato</t>
-  </si>
-  <si>
-    <t>temi presenti in percezione</t>
-  </si>
-  <si>
-    <t>temi presenti in totale</t>
-  </si>
-  <si>
-    <t>temi deboli in risultato</t>
-  </si>
-  <si>
-    <t>temi deboli in percezione</t>
-  </si>
-  <si>
-    <t>temi deboli in totale</t>
-  </si>
-  <si>
-    <t>temi presenti in intenzioni, risultato e percezioni</t>
-  </si>
-  <si>
-    <t>temi presenti o deboli in totale</t>
-  </si>
-  <si>
-    <t>temi presenti o deboli in intenzioni, risultato e percezioni</t>
-  </si>
-  <si>
-    <t>temi presenti in intenzioni e risultato</t>
-  </si>
-  <si>
-    <t>temi presenti o deboli in intenzioni e risultato</t>
-  </si>
-  <si>
-    <t>temi presenti in risultato e percezione</t>
-  </si>
-  <si>
-    <t>temi presenti o deboli in risultato e percezione</t>
-  </si>
-  <si>
-    <t>Punteggio di genere</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>Condizione</t>
-  </si>
-  <si>
     <t>Realtà/Finzione</t>
   </si>
   <si>
@@ -222,7 +171,34 @@
     <t>&gt;</t>
   </si>
   <si>
-    <t>correlazione</t>
+    <t>Utilizzo</t>
+  </si>
+  <si>
+    <t>Coerenza</t>
+  </si>
+  <si>
+    <t>camera a mano</t>
+  </si>
+  <si>
+    <t>sguardi in camera</t>
+  </si>
+  <si>
+    <t>interviste</t>
+  </si>
+  <si>
+    <t>voce fuori campo</t>
+  </si>
+  <si>
+    <t>found footage</t>
+  </si>
+  <si>
+    <t>elemento caratteristico</t>
+  </si>
+  <si>
+    <t>Punteggio pubblico</t>
+  </si>
+  <si>
+    <t>Punteggio tecnico</t>
   </si>
 </sst>
 </file>
@@ -272,9 +248,6 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -282,6 +255,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2311,7 +2287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBE84FA-B676-46CE-BED0-D965D08D268D}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -2327,16 +2303,16 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2344,476 +2320,476 @@
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>59</v>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>61</v>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>60</v>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>60</v>
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>60</v>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>61</v>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>60</v>
+      <c r="B8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>60</v>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>59</v>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>61</v>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>61</v>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>59</v>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>61</v>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>61</v>
+      <c r="B15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>60</v>
+      <c r="B16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>60</v>
+      <c r="B17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>60</v>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>61</v>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>59</v>
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>59</v>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>60</v>
+      <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>59</v>
+      <c r="B23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>59</v>
+      <c r="B24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>60</v>
+      <c r="B25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>60</v>
+      <c r="B26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>59</v>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>60</v>
+      <c r="B28" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>59</v>
+      <c r="B29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2825,7 +2801,534 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8187EC30-3A32-4FED-98FF-09F7642779C9}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8616C4-D75F-42DC-9983-BE1C4421A63A}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -2833,233 +3336,96 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8616C4-D75F-42DC-9983-BE1C4421A63A}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="5">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>1.54</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="5">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>2.93</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="5">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="5">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>4.6100000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="5">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>3.46</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="5">
+        <v>3.23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>4.53</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>